<commit_message>
Added Task1 - Polinomial class
</commit_message>
<xml_diff>
--- a/NET.S.2018.Ganko.05/Task1/Таблица сравнения ссылочных и значимых типов.xlsx
+++ b/NET.S.2018.Ganko.05/Task1/Таблица сравнения ссылочных и значимых типов.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Признаки для сравнения</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>При копировании переменной ссылочного типа, копируется значение ссылки. Т.е. мы получаем две ссылки указывающие на единственный объект в куче.</t>
+  </si>
+  <si>
+    <t>Все значимые типы являются неявно запечатанными и не участвуют в наследовании. Но значимые типы могу реализовывать интерфейсы в любом количестве. Значимые типы опосредовано производные от System.Object через System.ValueType</t>
+  </si>
+  <si>
+    <t>Все ссылочные типы являются производным от типа System.Object. C# поддерживает только единичное наследование классов. Ссылочные типы могут реализовывать интерфейсы в любом количестве.</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -555,8 +561,12 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>

</xml_diff>